<commit_message>
Acrescentando prints para documentação
</commit_message>
<xml_diff>
--- a/Banco de Dados/Tabelas - WishList.xlsx
+++ b/Banco de Dados/Tabelas - WishList.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SelmaeCândida\Downloads\SENAI-PROGRAMAÇÃO\WishList\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\43765601896\Downloads\senai-wishlist-desafio\Banco de Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7752" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Verbos" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Id</t>
   </si>
@@ -50,13 +50,94 @@
   </si>
   <si>
     <t>Id_Verbo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comprar </t>
+  </si>
+  <si>
+    <t>Ganhar</t>
+  </si>
+  <si>
+    <t>Viajar</t>
+  </si>
+  <si>
+    <t>Morar</t>
+  </si>
+  <si>
+    <t>Outros</t>
+  </si>
+  <si>
+    <t>Sem categoria</t>
+  </si>
+  <si>
+    <t>Querer</t>
+  </si>
+  <si>
+    <t>Vencer</t>
+  </si>
+  <si>
+    <t>Perder</t>
+  </si>
+  <si>
+    <t>Ariel</t>
+  </si>
+  <si>
+    <t>Cândida</t>
+  </si>
+  <si>
+    <t>Enzo</t>
+  </si>
+  <si>
+    <t>ariel</t>
+  </si>
+  <si>
+    <t>candida</t>
+  </si>
+  <si>
+    <t>enzo</t>
+  </si>
+  <si>
+    <t>ariel@gmail.com</t>
+  </si>
+  <si>
+    <t>candida@gmail.com</t>
+  </si>
+  <si>
+    <t>enzo@gmail.com</t>
+  </si>
+  <si>
+    <t>Comprar PC da NASA.</t>
+  </si>
+  <si>
+    <t>Não sei o que desejar!</t>
+  </si>
+  <si>
+    <t>Ser famoso.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comprar um caminhão. </t>
+  </si>
+  <si>
+    <t>Comprar um triciclo.</t>
+  </si>
+  <si>
+    <t>Viajar para Ubatuba.</t>
+  </si>
+  <si>
+    <t>VERBOS</t>
+  </si>
+  <si>
+    <t>USUÁRIOS</t>
+  </si>
+  <si>
+    <t>DESEJOS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,13 +152,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -104,10 +205,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -115,8 +217,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -135,7 +250,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -173,7 +288,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -245,7 +360,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -395,132 +510,359 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="14.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="2.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C5" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="2.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="4">
+        <v>43562</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="4">
+        <v>43561</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="4">
+        <v>43378</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="4">
+        <v>43449</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="4">
+        <v>42736</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="4">
+        <v>42860</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>